<commit_message>
Add mass spectra to Excel file
</commit_message>
<xml_diff>
--- a/docs/examples/IsotopeRangeExample2.xlsx
+++ b/docs/examples/IsotopeRangeExample2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Projects\SangtaeKim\MSGFPlus\docs\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B730DFD-181C-4CE7-98FE-C0611F9B4008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12848123-E52D-48A1-B699-2B085957695F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="19932" windowHeight="10872" xr2:uid="{BA7180DC-7D38-48F8-A0DE-924D81004E4A}"/>
+    <workbookView xWindow="1968" yWindow="732" windowWidth="19932" windowHeight="10872" xr2:uid="{BA7180DC-7D38-48F8-A0DE-924D81004E4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Theoretical m/z</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Correct Mass Error (ppm)</t>
+  </si>
+  <si>
+    <t>Values highlighted in green satisfy "IsotopeErrorRange=0,1" and "PrecursorMassTolerance=20ppm"</t>
   </si>
 </sst>
 </file>
@@ -92,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -111,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,7 +123,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -166,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -183,13 +192,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -216,10 +225,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -228,6 +239,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -237,6 +253,85 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{815BDD78-6108-46C0-9ACF-7AEFE286D614}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5913120" y="1889760"/>
+          <a:ext cx="10744200" cy="5006340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,23 +631,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5ABCF3-2769-4960-8D71-7F15233AA3DF}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -560,15 +655,18 @@
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -576,7 +674,7 @@
         <v>1.00727649</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="F4" s="14" t="s">
         <v>15</v>
       </c>
@@ -590,7 +688,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="16"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
@@ -635,7 +733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f>B6+$B$1</f>
         <v>637.83500000000004</v>
@@ -659,7 +757,7 @@
         <f>ABS($D6 - $C6 - F$5 * 1.00335)</f>
         <v>1.0133499999999909</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="19">
         <f t="shared" ref="G6:I7" si="1">ABS($D6 - $C6 - G$5 * 1.00335)</f>
         <v>9.9999999999909051E-3</v>
       </c>
@@ -675,7 +773,7 @@
         <f>F6 * 1000000 / $C6</f>
         <v>795.62333939759651</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="20">
         <f t="shared" ref="K6:M7" si="2">G6 * 1000000 / $C6</f>
         <v>7.8514169773215574</v>
       </c>
@@ -688,7 +786,7 @@
         <v>1567.6924278632284</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f>A6</f>
         <v>637.83500000000004</v>
@@ -716,7 +814,7 @@
         <f t="shared" si="1"/>
         <v>1.0099999999999909</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="19">
         <f t="shared" si="1"/>
         <v>6.6499999999909409E-3</v>
       </c>
@@ -732,7 +830,7 @@
         <f t="shared" si="2"/>
         <v>792.99311471019143</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="20">
         <f t="shared" si="2"/>
         <v>5.2211922899164716</v>
       </c>
@@ -741,7 +839,7 @@
         <v>782.55073013035849</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
@@ -756,7 +854,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f>B9+$B$1</f>
         <v>607.29499999999996</v>
@@ -780,7 +878,7 @@
         <f>ABS($D9 - $C9 - F$5 * 1.00335)</f>
         <v>1.0133499999999909</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="19">
         <f t="shared" ref="G9:I10" si="3">ABS($D9 - $C9 - G$5 * 1.00335)</f>
         <v>9.9999999999909051E-3</v>
       </c>
@@ -796,7 +894,7 @@
         <f>F9 * 1000000 / $C9</f>
         <v>835.70057639743482</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="20">
         <f t="shared" ref="K9:M10" si="4">G9 * 1000000 / $C9</f>
         <v>8.2469095218501227</v>
       </c>
@@ -809,7 +907,7 @@
         <v>1646.6604242293192</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f>A9</f>
         <v>607.29499999999996</v>
@@ -837,7 +935,7 @@
         <f t="shared" si="3"/>
         <v>0.99000000000000909</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="19">
         <f t="shared" si="3"/>
         <v>1.3349999999990869E-2</v>
       </c>
@@ -853,7 +951,7 @@
         <f t="shared" si="4"/>
         <v>816.44404266391223</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="20">
         <f t="shared" si="4"/>
         <v>11.009624211672397</v>
       </c>
@@ -862,40 +960,606 @@
         <v>838.46329108725695</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="17"/>
+      <c r="X22" s="17"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+    </row>
+    <row r="33" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+    </row>
+    <row r="34" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+    </row>
+    <row r="35" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+    </row>
+    <row r="36" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+    </row>
+    <row r="37" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+    </row>
+    <row r="38" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="17"/>
+    </row>
+    <row r="39" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+    </row>
+    <row r="40" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+      <c r="V40" s="18"/>
+      <c r="W40" s="18"/>
+      <c r="X40" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -903,5 +1567,6 @@
     <mergeCell ref="J4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>